<commit_message>
more data + descriptions
</commit_message>
<xml_diff>
--- a/Data/Mystic_MAG_Quality_Stats.xlsx
+++ b/Data/Mystic_MAG_Quality_Stats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="123">
   <si>
     <t>Unbinned</t>
   </si>
@@ -753,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6FFC79D-6405-2341-B772-E5F9363F8E34}">
-  <dimension ref="A1:W89"/>
+  <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -768,7 +768,7 @@
     <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:22">
       <c r="B1" t="s">
         <v>88</v>
       </c>
@@ -809,34 +809,31 @@
         <v>118</v>
       </c>
       <c r="O1" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="P1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="R1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="T1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V1" t="s">
-        <v>111</v>
-      </c>
-      <c r="W1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -903,11 +900,8 @@
       <c r="V2" t="s">
         <v>108</v>
       </c>
-      <c r="W2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23">
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -951,34 +945,31 @@
         <v>0.91909366674000004</v>
       </c>
       <c r="O3">
-        <v>0.66984268900999999</v>
+        <v>1.5773848717200001E-2</v>
       </c>
       <c r="P3">
-        <v>1.5773848717200001E-2</v>
+        <v>3966488</v>
       </c>
       <c r="Q3">
-        <v>3966488</v>
+        <v>130572</v>
       </c>
       <c r="R3">
-        <v>130572</v>
+        <v>146734</v>
       </c>
       <c r="S3">
-        <v>146734</v>
+        <v>22394.734463299999</v>
       </c>
       <c r="T3">
-        <v>22394.734463299999</v>
+        <v>30278.534351099999</v>
       </c>
       <c r="U3">
-        <v>30278.534351099999</v>
+        <v>35431</v>
       </c>
       <c r="V3">
-        <v>35431</v>
-      </c>
-      <c r="W3">
         <v>55351</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1022,34 +1013,31 @@
         <v>0.935218344699</v>
       </c>
       <c r="O4">
-        <v>0.59598164809999998</v>
+        <v>1.61015589744E-2</v>
       </c>
       <c r="P4">
-        <v>1.61015589744E-2</v>
+        <v>4828512</v>
       </c>
       <c r="Q4">
-        <v>4828512</v>
+        <v>179935</v>
       </c>
       <c r="R4">
-        <v>179935</v>
+        <v>210145</v>
       </c>
       <c r="S4">
-        <v>210145</v>
+        <v>11978.665012400001</v>
       </c>
       <c r="T4">
-        <v>11978.665012400001</v>
+        <v>13955.2369942</v>
       </c>
       <c r="U4">
-        <v>13955.2369942</v>
+        <v>20142</v>
       </c>
       <c r="V4">
-        <v>20142</v>
-      </c>
-      <c r="W4">
         <v>22485</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1093,34 +1081,31 @@
         <v>0.89161690671799998</v>
       </c>
       <c r="O5">
-        <v>0.46491991903800001</v>
+        <v>1.9764105846799999E-2</v>
       </c>
       <c r="P5">
-        <v>1.9764105846799999E-2</v>
+        <v>4649489</v>
       </c>
       <c r="Q5">
-        <v>4649489</v>
+        <v>23018</v>
       </c>
       <c r="R5">
         <v>23018</v>
       </c>
       <c r="S5">
-        <v>23018</v>
+        <v>4907.7180570199998</v>
       </c>
       <c r="T5">
-        <v>4907.7180570199998</v>
+        <v>5495.8498817999998</v>
       </c>
       <c r="U5">
-        <v>5495.8498817999998</v>
+        <v>6758</v>
       </c>
       <c r="V5">
-        <v>6758</v>
-      </c>
-      <c r="W5">
         <v>7413</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1164,34 +1149,31 @@
         <v>0.92834138118200005</v>
       </c>
       <c r="O6">
-        <v>0.603974489595</v>
+        <v>1.9064287304000001E-2</v>
       </c>
       <c r="P6">
-        <v>1.9064287304000001E-2</v>
+        <v>3281001</v>
       </c>
       <c r="Q6">
-        <v>3281001</v>
+        <v>88078</v>
       </c>
       <c r="R6">
-        <v>88078</v>
+        <v>88512</v>
       </c>
       <c r="S6">
-        <v>88512</v>
+        <v>5759.6678383099998</v>
       </c>
       <c r="T6">
-        <v>5759.6678383099998</v>
+        <v>6408.2050781199996</v>
       </c>
       <c r="U6">
-        <v>6408.2050781199996</v>
+        <v>12342</v>
       </c>
       <c r="V6">
-        <v>12342</v>
-      </c>
-      <c r="W6">
         <v>15021</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1235,34 +1217,31 @@
         <v>0.91130940360900003</v>
       </c>
       <c r="O7">
-        <v>0.44179514080499999</v>
+        <v>2.8055762839099999E-2</v>
       </c>
       <c r="P7">
-        <v>2.8055762839099999E-2</v>
+        <v>4214201</v>
       </c>
       <c r="Q7">
-        <v>4214201</v>
+        <v>40903</v>
       </c>
       <c r="R7">
         <v>40903</v>
       </c>
       <c r="S7">
-        <v>40903</v>
+        <v>6630.1118110199995</v>
       </c>
       <c r="T7">
-        <v>6630.1118110199995</v>
+        <v>7525.35892857</v>
       </c>
       <c r="U7">
-        <v>7525.35892857</v>
+        <v>9612</v>
       </c>
       <c r="V7">
-        <v>9612</v>
-      </c>
-      <c r="W7">
         <v>11587</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1306,34 +1285,31 @@
         <v>0.95992210575100001</v>
       </c>
       <c r="O8">
-        <v>0.46929806773100002</v>
+        <v>1.04896582235E-2</v>
       </c>
       <c r="P8">
-        <v>1.04896582235E-2</v>
+        <v>1381360</v>
       </c>
       <c r="Q8">
-        <v>1381360</v>
+        <v>118025</v>
       </c>
       <c r="R8">
         <v>118025</v>
       </c>
       <c r="S8">
-        <v>118025</v>
+        <v>20608.358209000002</v>
       </c>
       <c r="T8">
-        <v>20608.358209000002</v>
+        <v>22645.245901599999</v>
       </c>
       <c r="U8">
-        <v>22645.245901599999</v>
+        <v>36843</v>
       </c>
       <c r="V8">
         <v>36843</v>
       </c>
-      <c r="W8">
-        <v>36843</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23">
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1377,34 +1353,31 @@
         <v>0.94704186075600005</v>
       </c>
       <c r="O9">
-        <v>0.47138549167999999</v>
+        <v>1.3411320232499999E-2</v>
       </c>
       <c r="P9">
-        <v>1.3411320232499999E-2</v>
+        <v>1820249</v>
       </c>
       <c r="Q9">
-        <v>1820249</v>
+        <v>42015</v>
       </c>
       <c r="R9">
-        <v>42015</v>
+        <v>61423</v>
       </c>
       <c r="S9">
-        <v>61423</v>
+        <v>7809.2231759699998</v>
       </c>
       <c r="T9">
-        <v>7809.2231759699998</v>
+        <v>9146.9798995000001</v>
       </c>
       <c r="U9">
-        <v>9146.9798995000001</v>
+        <v>11293</v>
       </c>
       <c r="V9">
-        <v>11293</v>
-      </c>
-      <c r="W9">
         <v>13379</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:22">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1448,34 +1421,31 @@
         <v>0.92370263396499996</v>
       </c>
       <c r="O10">
-        <v>0.50994835892099999</v>
+        <v>2.7685678658E-2</v>
       </c>
       <c r="P10">
-        <v>2.7685678658E-2</v>
+        <v>2165291</v>
       </c>
       <c r="Q10">
-        <v>2165291</v>
+        <v>28252</v>
       </c>
       <c r="R10">
         <v>28252</v>
       </c>
       <c r="S10">
-        <v>28252</v>
+        <v>4093.7210626199999</v>
       </c>
       <c r="T10">
-        <v>4093.7210626199999</v>
+        <v>4932.3257403199996</v>
       </c>
       <c r="U10">
-        <v>4932.3257403199996</v>
+        <v>5305</v>
       </c>
       <c r="V10">
-        <v>5305</v>
-      </c>
-      <c r="W10">
         <v>6196</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:22">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1519,34 +1489,31 @@
         <v>0.928244326811</v>
       </c>
       <c r="O11">
-        <v>0.63054505387699999</v>
+        <v>1.60825010521E-2</v>
       </c>
       <c r="P11">
-        <v>1.60825010521E-2</v>
+        <v>3346927</v>
       </c>
       <c r="Q11">
-        <v>3346927</v>
+        <v>65635</v>
       </c>
       <c r="R11">
-        <v>65635</v>
+        <v>85669</v>
       </c>
       <c r="S11">
-        <v>85669</v>
+        <v>8382.5100502500009</v>
       </c>
       <c r="T11">
-        <v>8382.5100502500009</v>
+        <v>11702.541958</v>
       </c>
       <c r="U11">
-        <v>11702.541958</v>
+        <v>16063</v>
       </c>
       <c r="V11">
-        <v>16063</v>
-      </c>
-      <c r="W11">
         <v>23584</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:22">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1590,34 +1557,31 @@
         <v>0.90233821165500006</v>
       </c>
       <c r="O12">
-        <v>0.48724171378199999</v>
+        <v>2.6732935238000001E-2</v>
       </c>
       <c r="P12">
-        <v>2.6732935238000001E-2</v>
+        <v>4428641</v>
       </c>
       <c r="Q12">
-        <v>4428641</v>
+        <v>37902</v>
       </c>
       <c r="R12">
         <v>37902</v>
       </c>
       <c r="S12">
-        <v>37902</v>
+        <v>5750.6298701300002</v>
       </c>
       <c r="T12">
-        <v>5750.6298701300002</v>
+        <v>6116.9074585600001</v>
       </c>
       <c r="U12">
-        <v>6116.9074585600001</v>
+        <v>7700</v>
       </c>
       <c r="V12">
-        <v>7700</v>
-      </c>
-      <c r="W12">
         <v>8048</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:22">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1661,34 +1625,31 @@
         <v>0.94736851756100005</v>
       </c>
       <c r="O13">
-        <v>0.62830377592700004</v>
+        <v>3.9496225203499997E-2</v>
       </c>
       <c r="P13">
-        <v>3.9496225203499997E-2</v>
+        <v>1090716</v>
       </c>
       <c r="Q13">
-        <v>1090716</v>
+        <v>58732</v>
       </c>
       <c r="R13">
         <v>58732</v>
       </c>
       <c r="S13">
-        <v>58732</v>
+        <v>5832.3315507999996</v>
       </c>
       <c r="T13">
-        <v>5832.3315507999996</v>
+        <v>6059.5333333299996</v>
       </c>
       <c r="U13">
-        <v>6059.5333333299996</v>
+        <v>13683</v>
       </c>
       <c r="V13">
         <v>13683</v>
       </c>
-      <c r="W13">
-        <v>13683</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23">
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1732,34 +1693,31 @@
         <v>0.91818257392400005</v>
       </c>
       <c r="O14">
-        <v>0.39955343149299999</v>
+        <v>1.4218957667099999E-2</v>
       </c>
       <c r="P14">
-        <v>1.4218957667099999E-2</v>
+        <v>3079454</v>
       </c>
       <c r="Q14">
-        <v>3079454</v>
+        <v>301284</v>
       </c>
       <c r="R14">
         <v>301284</v>
       </c>
       <c r="S14">
-        <v>301284</v>
+        <v>46645.257575800002</v>
       </c>
       <c r="T14">
-        <v>46645.257575800002</v>
+        <v>59220.269230799997</v>
       </c>
       <c r="U14">
-        <v>59220.269230799997</v>
+        <v>86512</v>
       </c>
       <c r="V14">
-        <v>86512</v>
-      </c>
-      <c r="W14">
         <v>133765</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:22">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1803,34 +1761,31 @@
         <v>0.915196280571</v>
       </c>
       <c r="O15">
-        <v>0.50278778921</v>
+        <v>3.2279854645400001E-2</v>
       </c>
       <c r="P15">
-        <v>3.2279854645400001E-2</v>
+        <v>1792103</v>
       </c>
       <c r="Q15">
-        <v>1792103</v>
+        <v>17972</v>
       </c>
       <c r="R15">
         <v>17972</v>
       </c>
       <c r="S15">
-        <v>17972</v>
+        <v>2366.66182299</v>
       </c>
       <c r="T15">
-        <v>2366.66182299</v>
+        <v>2549.2219061199999</v>
       </c>
       <c r="U15">
-        <v>2549.2219061199999</v>
+        <v>2727</v>
       </c>
       <c r="V15">
-        <v>2727</v>
-      </c>
-      <c r="W15">
         <v>2839</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:22">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1874,34 +1829,31 @@
         <v>0.89254281664699997</v>
       </c>
       <c r="O16">
-        <v>0.41624468580700003</v>
+        <v>1.8259419879999999E-2</v>
       </c>
       <c r="P16">
-        <v>1.8259419879999999E-2</v>
+        <v>2531492</v>
       </c>
       <c r="Q16">
-        <v>2531492</v>
+        <v>98129</v>
       </c>
       <c r="R16">
         <v>98129</v>
       </c>
       <c r="S16">
-        <v>98129</v>
+        <v>15621.7469136</v>
       </c>
       <c r="T16">
-        <v>15621.7469136</v>
+        <v>16989.879194599998</v>
       </c>
       <c r="U16">
-        <v>16989.879194599998</v>
+        <v>27954</v>
       </c>
       <c r="V16">
-        <v>27954</v>
-      </c>
-      <c r="W16">
         <v>29416</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:22">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1945,34 +1897,31 @@
         <v>0.91101648654699996</v>
       </c>
       <c r="O17">
-        <v>0.62704914196600003</v>
+        <v>2.1765988064599999E-2</v>
       </c>
       <c r="P17">
-        <v>2.1765988064599999E-2</v>
+        <v>3526451</v>
       </c>
       <c r="Q17">
-        <v>3526451</v>
+        <v>142856</v>
       </c>
       <c r="R17">
         <v>142856</v>
       </c>
       <c r="S17">
-        <v>142856</v>
+        <v>4485.4465648900004</v>
       </c>
       <c r="T17">
-        <v>4485.4465648900004</v>
+        <v>4771.92286874</v>
       </c>
       <c r="U17">
-        <v>4771.92286874</v>
+        <v>36613</v>
       </c>
       <c r="V17">
-        <v>36613</v>
-      </c>
-      <c r="W17">
         <v>38816</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:22">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2016,34 +1965,31 @@
         <v>0.93798388939699995</v>
       </c>
       <c r="O18">
-        <v>0.45444325344999997</v>
+        <v>2.0734241355800001E-2</v>
       </c>
       <c r="P18">
-        <v>2.0734241355800001E-2</v>
+        <v>4931783</v>
       </c>
       <c r="Q18">
-        <v>4931783</v>
+        <v>108208</v>
       </c>
       <c r="R18">
-        <v>108208</v>
+        <v>115085</v>
       </c>
       <c r="S18">
-        <v>115085</v>
+        <v>10064.1918367</v>
       </c>
       <c r="T18">
-        <v>10064.1918367</v>
+        <v>10583.225321899999</v>
       </c>
       <c r="U18">
-        <v>10583.225321899999</v>
+        <v>19664</v>
       </c>
       <c r="V18">
-        <v>19664</v>
-      </c>
-      <c r="W18">
         <v>21197</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:22">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2087,34 +2033,31 @@
         <v>0.89910769362800003</v>
       </c>
       <c r="O19">
-        <v>0.62970345205</v>
+        <v>2.4788870453499999E-2</v>
       </c>
       <c r="P19">
-        <v>2.4788870453499999E-2</v>
+        <v>7269028</v>
       </c>
       <c r="Q19">
-        <v>7269028</v>
+        <v>32308</v>
       </c>
       <c r="R19">
-        <v>32308</v>
+        <v>32608</v>
       </c>
       <c r="S19">
-        <v>32608</v>
+        <v>3548.4321289099998</v>
       </c>
       <c r="T19">
-        <v>3548.4321289099998</v>
+        <v>3733.45043657</v>
       </c>
       <c r="U19">
-        <v>3733.45043657</v>
+        <v>4193</v>
       </c>
       <c r="V19">
-        <v>4193</v>
-      </c>
-      <c r="W19">
         <v>4295</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:22">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -2158,34 +2101,31 @@
         <v>0.87213825768700004</v>
       </c>
       <c r="O20">
-        <v>0.65315038368</v>
+        <v>1.8038554869600001E-2</v>
       </c>
       <c r="P20">
-        <v>1.8038554869600001E-2</v>
+        <v>5905668</v>
       </c>
       <c r="Q20">
-        <v>5905668</v>
+        <v>45065</v>
       </c>
       <c r="R20">
-        <v>45065</v>
+        <v>49379</v>
       </c>
       <c r="S20">
-        <v>49379</v>
+        <v>4598.2383177600004</v>
       </c>
       <c r="T20">
-        <v>4598.2383177600004</v>
+        <v>5180.4105263199999</v>
       </c>
       <c r="U20">
-        <v>5180.4105263199999</v>
+        <v>6782</v>
       </c>
       <c r="V20">
-        <v>6782</v>
-      </c>
-      <c r="W20">
         <v>7494</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:22">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2229,34 +2169,31 @@
         <v>0.90386609266200002</v>
       </c>
       <c r="O21">
-        <v>0.50595835578699999</v>
+        <v>1.5828429204299999E-2</v>
       </c>
       <c r="P21">
-        <v>1.5828429204299999E-2</v>
+        <v>1540289</v>
       </c>
       <c r="Q21">
-        <v>1540289</v>
+        <v>47929</v>
       </c>
       <c r="R21">
         <v>47929</v>
       </c>
       <c r="S21">
-        <v>47929</v>
+        <v>9006.9590643299998</v>
       </c>
       <c r="T21">
-        <v>9006.9590643299998</v>
+        <v>9060.5235294100003</v>
       </c>
       <c r="U21">
-        <v>9060.5235294100003</v>
+        <v>16626</v>
       </c>
       <c r="V21">
-        <v>16626</v>
-      </c>
-      <c r="W21">
         <v>16683</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:22">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2300,34 +2237,31 @@
         <v>0.93572908565599999</v>
       </c>
       <c r="O22">
-        <v>0.62034825955399997</v>
+        <v>1.6071386658200001E-2</v>
       </c>
       <c r="P22">
-        <v>1.6071386658200001E-2</v>
+        <v>3523180</v>
       </c>
       <c r="Q22">
-        <v>3523180</v>
+        <v>57075</v>
       </c>
       <c r="R22">
         <v>57075</v>
       </c>
       <c r="S22">
-        <v>57075</v>
+        <v>6475.47794118</v>
       </c>
       <c r="T22">
-        <v>6475.47794118</v>
+        <v>6908.1960784299999</v>
       </c>
       <c r="U22">
-        <v>6908.1960784299999</v>
+        <v>9969</v>
       </c>
       <c r="V22">
-        <v>9969</v>
-      </c>
-      <c r="W22">
         <v>11077</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:22">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2371,34 +2305,31 @@
         <v>0.94959927890600004</v>
       </c>
       <c r="O23">
-        <v>0.43685820843700002</v>
+        <v>1.1574283834899999E-2</v>
       </c>
       <c r="P23">
-        <v>1.1574283834899999E-2</v>
+        <v>1225915</v>
       </c>
       <c r="Q23">
-        <v>1225915</v>
+        <v>123094</v>
       </c>
       <c r="R23">
-        <v>123094</v>
+        <v>143326</v>
       </c>
       <c r="S23">
-        <v>143326</v>
+        <v>16320.2</v>
       </c>
       <c r="T23">
-        <v>16320.2</v>
+        <v>21891.3392857</v>
       </c>
       <c r="U23">
-        <v>21891.3392857</v>
+        <v>32728</v>
       </c>
       <c r="V23">
-        <v>32728</v>
-      </c>
-      <c r="W23">
         <v>58485</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:22">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -2442,34 +2373,31 @@
         <v>0.91458544803399999</v>
       </c>
       <c r="O24">
-        <v>0.638429060085</v>
+        <v>2.53240606689E-2</v>
       </c>
       <c r="P24">
-        <v>2.53240606689E-2</v>
+        <v>4524873</v>
       </c>
       <c r="Q24">
-        <v>4524873</v>
+        <v>11217</v>
       </c>
       <c r="R24">
         <v>11217</v>
       </c>
       <c r="S24">
-        <v>11217</v>
+        <v>2251.60925834</v>
       </c>
       <c r="T24">
-        <v>2251.60925834</v>
+        <v>2340.8551474400001</v>
       </c>
       <c r="U24">
-        <v>2340.8551474400001</v>
+        <v>2576</v>
       </c>
       <c r="V24">
-        <v>2576</v>
-      </c>
-      <c r="W24">
         <v>2687</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:22">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -2513,34 +2441,31 @@
         <v>0.93363022144300001</v>
       </c>
       <c r="O25">
-        <v>0.65336259098399996</v>
+        <v>2.4629234942500002E-2</v>
       </c>
       <c r="P25">
-        <v>2.4629234942500002E-2</v>
+        <v>1962580</v>
       </c>
       <c r="Q25">
-        <v>1962580</v>
+        <v>37481</v>
       </c>
       <c r="R25">
-        <v>37481</v>
+        <v>40480</v>
       </c>
       <c r="S25">
-        <v>40480</v>
+        <v>2640.4845222099998</v>
       </c>
       <c r="T25">
-        <v>2640.4845222099998</v>
+        <v>2666.5489130400001</v>
       </c>
       <c r="U25">
-        <v>2666.5489130400001</v>
+        <v>3012</v>
       </c>
       <c r="V25">
-        <v>3012</v>
-      </c>
-      <c r="W25">
         <v>3087</v>
       </c>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:22">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -2584,34 +2509,31 @@
         <v>0.94176283216699996</v>
       </c>
       <c r="O26">
-        <v>0.53211832467200004</v>
+        <v>1.7725453294699999E-2</v>
       </c>
       <c r="P26">
-        <v>1.7725453294699999E-2</v>
+        <v>2387204</v>
       </c>
       <c r="Q26">
-        <v>2387204</v>
+        <v>23967</v>
       </c>
       <c r="R26">
         <v>23967</v>
       </c>
       <c r="S26">
-        <v>23967</v>
+        <v>3371.3615819199999</v>
       </c>
       <c r="T26">
-        <v>3371.3615819199999</v>
+        <v>3510.59411765</v>
       </c>
       <c r="U26">
-        <v>3510.59411765</v>
+        <v>4545</v>
       </c>
       <c r="V26">
-        <v>4545</v>
-      </c>
-      <c r="W26">
         <v>4725</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:22">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2655,34 +2577,31 @@
         <v>0.87929750329300005</v>
       </c>
       <c r="O27">
-        <v>0.48072265053500002</v>
+        <v>2.1243149515899999E-2</v>
       </c>
       <c r="P27">
-        <v>2.1243149515899999E-2</v>
+        <v>4603865</v>
       </c>
       <c r="Q27">
-        <v>4603865</v>
+        <v>60858</v>
       </c>
       <c r="R27">
         <v>60858</v>
       </c>
       <c r="S27">
-        <v>60858</v>
+        <v>7007.1826484000003</v>
       </c>
       <c r="T27">
-        <v>7007.1826484000003</v>
+        <v>7148.8586956500003</v>
       </c>
       <c r="U27">
-        <v>7148.8586956500003</v>
+        <v>13676</v>
       </c>
       <c r="V27">
-        <v>13676</v>
-      </c>
-      <c r="W27">
         <v>13926</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:22">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2726,34 +2645,31 @@
         <v>0.88436973271499997</v>
       </c>
       <c r="O28">
-        <v>0.50767509258200005</v>
+        <v>3.7000253946199997E-2</v>
       </c>
       <c r="P28">
-        <v>3.7000253946199997E-2</v>
+        <v>4516084</v>
       </c>
       <c r="Q28">
-        <v>4516084</v>
+        <v>180428</v>
       </c>
       <c r="R28">
-        <v>180428</v>
+        <v>240506</v>
       </c>
       <c r="S28">
-        <v>240506</v>
+        <v>48556.0322581</v>
       </c>
       <c r="T28">
-        <v>48556.0322581</v>
+        <v>60214.4533333</v>
       </c>
       <c r="U28">
-        <v>60214.4533333</v>
+        <v>100999</v>
       </c>
       <c r="V28">
-        <v>100999</v>
-      </c>
-      <c r="W28">
         <v>118629</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:22">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2797,34 +2713,31 @@
         <v>0.91950124395599997</v>
       </c>
       <c r="O29">
-        <v>0.36204939356400001</v>
+        <v>3.2755095637199999E-2</v>
       </c>
       <c r="P29">
-        <v>3.2755095637199999E-2</v>
+        <v>2624289</v>
       </c>
       <c r="Q29">
-        <v>2624289</v>
+        <v>33667</v>
       </c>
       <c r="R29">
         <v>33667</v>
       </c>
       <c r="S29">
-        <v>33667</v>
+        <v>3531.9905787299999</v>
       </c>
       <c r="T29">
-        <v>3531.9905787299999</v>
+        <v>3541.5506072899998</v>
       </c>
       <c r="U29">
-        <v>3541.5506072899998</v>
+        <v>4889</v>
       </c>
       <c r="V29">
         <v>4889</v>
       </c>
-      <c r="W29">
-        <v>4889</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23">
+    </row>
+    <row r="30" spans="1:22">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2868,34 +2781,31 @@
         <v>0.92689640891799996</v>
       </c>
       <c r="O30">
-        <v>0.70113234678000003</v>
+        <v>3.2291846314900001E-2</v>
       </c>
       <c r="P30">
-        <v>3.2291846314900001E-2</v>
+        <v>9001856</v>
       </c>
       <c r="Q30">
-        <v>9001856</v>
+        <v>31303</v>
       </c>
       <c r="R30">
         <v>31303</v>
       </c>
       <c r="S30">
-        <v>31303</v>
+        <v>4129.8806792100004</v>
       </c>
       <c r="T30">
-        <v>4129.8806792100004</v>
+        <v>4268.3053579899997</v>
       </c>
       <c r="U30">
-        <v>4268.3053579899997</v>
+        <v>5858</v>
       </c>
       <c r="V30">
-        <v>5858</v>
-      </c>
-      <c r="W30">
         <v>6049</v>
       </c>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:22">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2939,34 +2849,31 @@
         <v>0.93334032696900004</v>
       </c>
       <c r="O31">
-        <v>0.68837103725100002</v>
+        <v>3.1587626805399997E-2</v>
       </c>
       <c r="P31">
-        <v>3.1587626805399997E-2</v>
+        <v>2163872</v>
       </c>
       <c r="Q31">
-        <v>2163872</v>
+        <v>21179</v>
       </c>
       <c r="R31">
         <v>21179</v>
       </c>
       <c r="S31">
-        <v>21179</v>
+        <v>2831.2591622999998</v>
       </c>
       <c r="T31">
-        <v>2831.2591622999998</v>
+        <v>3039.1460674199998</v>
       </c>
       <c r="U31">
-        <v>3039.1460674199998</v>
+        <v>3451</v>
       </c>
       <c r="V31">
-        <v>3451</v>
-      </c>
-      <c r="W31">
         <v>3744</v>
       </c>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:22">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -3010,34 +2917,31 @@
         <v>0.92761254006899996</v>
       </c>
       <c r="O32">
-        <v>0.543998813887</v>
+        <v>1.7517665282000001E-2</v>
       </c>
       <c r="P32">
-        <v>1.7517665282000001E-2</v>
+        <v>1938554</v>
       </c>
       <c r="Q32">
-        <v>1938554</v>
+        <v>40603</v>
       </c>
       <c r="R32">
         <v>40603</v>
       </c>
       <c r="S32">
-        <v>40603</v>
+        <v>5795.6107784400001</v>
       </c>
       <c r="T32">
-        <v>5795.6107784400001</v>
+        <v>6571.3694915300002</v>
       </c>
       <c r="U32">
-        <v>6571.3694915300002</v>
+        <v>7813</v>
       </c>
       <c r="V32">
-        <v>7813</v>
-      </c>
-      <c r="W32">
         <v>9752</v>
       </c>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:22">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -3081,34 +2985,31 @@
         <v>0.88346397753600003</v>
       </c>
       <c r="O33">
-        <v>0.62924157093400002</v>
+        <v>3.4617391406099998E-2</v>
       </c>
       <c r="P33">
-        <v>3.4617391406099998E-2</v>
+        <v>3922358</v>
       </c>
       <c r="Q33">
-        <v>3922358</v>
+        <v>100990</v>
       </c>
       <c r="R33">
-        <v>100990</v>
+        <v>241511</v>
       </c>
       <c r="S33">
-        <v>241511</v>
+        <v>7386.5104364299996</v>
       </c>
       <c r="T33">
-        <v>7386.5104364299996</v>
+        <v>17668.279279300001</v>
       </c>
       <c r="U33">
-        <v>17668.279279300001</v>
+        <v>12772</v>
       </c>
       <c r="V33">
-        <v>12772</v>
-      </c>
-      <c r="W33">
         <v>44513</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:22">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -3152,34 +3053,31 @@
         <v>0.92722500900299998</v>
       </c>
       <c r="O34">
-        <v>0.42298856429699999</v>
+        <v>1.3382268530399999E-2</v>
       </c>
       <c r="P34">
-        <v>1.3382268530399999E-2</v>
+        <v>2749090</v>
       </c>
       <c r="Q34">
-        <v>2749090</v>
+        <v>82290</v>
       </c>
       <c r="R34">
         <v>82290</v>
       </c>
       <c r="S34">
-        <v>82290</v>
+        <v>13880.8585859</v>
       </c>
       <c r="T34">
-        <v>13880.8585859</v>
+        <v>15709.085714299999</v>
       </c>
       <c r="U34">
-        <v>15709.085714299999</v>
+        <v>22924</v>
       </c>
       <c r="V34">
-        <v>22924</v>
-      </c>
-      <c r="W34">
         <v>24107</v>
       </c>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:22">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -3223,34 +3121,31 @@
         <v>0.94377808234299998</v>
       </c>
       <c r="O35">
-        <v>0.53787306619099995</v>
+        <v>2.1418676391100001E-2</v>
       </c>
       <c r="P35">
-        <v>2.1418676391100001E-2</v>
+        <v>1651171</v>
       </c>
       <c r="Q35">
-        <v>1651171</v>
+        <v>17210</v>
       </c>
       <c r="R35">
         <v>17210</v>
       </c>
       <c r="S35">
-        <v>17210</v>
+        <v>2274.2162534399999</v>
       </c>
       <c r="T35">
-        <v>2274.2162534399999</v>
+        <v>2302.8884239899999</v>
       </c>
       <c r="U35">
-        <v>2302.8884239899999</v>
+        <v>2891</v>
       </c>
       <c r="V35">
-        <v>2891</v>
-      </c>
-      <c r="W35">
         <v>2904</v>
       </c>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:22">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -3294,34 +3189,31 @@
         <v>0.89379010100699996</v>
       </c>
       <c r="O36">
-        <v>0.49551036833200002</v>
+        <v>3.3247383525999999E-2</v>
       </c>
       <c r="P36">
-        <v>3.3247383525999999E-2</v>
+        <v>5676759</v>
       </c>
       <c r="Q36">
-        <v>5676759</v>
+        <v>26601</v>
       </c>
       <c r="R36">
-        <v>26601</v>
+        <v>50460</v>
       </c>
       <c r="S36">
-        <v>50460</v>
+        <v>3336.7101704900001</v>
       </c>
       <c r="T36">
-        <v>3336.7101704900001</v>
+        <v>3521.5626550900001</v>
       </c>
       <c r="U36">
-        <v>3521.5626550900001</v>
+        <v>4432</v>
       </c>
       <c r="V36">
-        <v>4432</v>
-      </c>
-      <c r="W36">
         <v>4547</v>
       </c>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:22">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -3365,34 +3257,31 @@
         <v>0.93953592104299999</v>
       </c>
       <c r="O37">
-        <v>0.36454982381500001</v>
+        <v>1.52667886418E-2</v>
       </c>
       <c r="P37">
-        <v>1.52667886418E-2</v>
+        <v>1591755</v>
       </c>
       <c r="Q37">
-        <v>1591755</v>
+        <v>14397</v>
       </c>
       <c r="R37">
-        <v>14397</v>
+        <v>22712</v>
       </c>
       <c r="S37">
-        <v>22712</v>
+        <v>2497.1036106800002</v>
       </c>
       <c r="T37">
-        <v>2497.1036106800002</v>
+        <v>2618.01809211</v>
       </c>
       <c r="U37">
-        <v>2618.01809211</v>
+        <v>2806</v>
       </c>
       <c r="V37">
-        <v>2806</v>
-      </c>
-      <c r="W37">
         <v>2953</v>
       </c>
     </row>
-    <row r="38" spans="1:23">
+    <row r="38" spans="1:22">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -3436,34 +3325,31 @@
         <v>0.92406938087699997</v>
       </c>
       <c r="O38">
-        <v>0.68060576562800001</v>
+        <v>1.6556945059699998E-2</v>
       </c>
       <c r="P38">
-        <v>1.6556945059699998E-2</v>
+        <v>2500862</v>
       </c>
       <c r="Q38">
-        <v>2500862</v>
+        <v>41302</v>
       </c>
       <c r="R38">
-        <v>41302</v>
+        <v>42381</v>
       </c>
       <c r="S38">
-        <v>42381</v>
+        <v>7413.6261127600001</v>
       </c>
       <c r="T38">
-        <v>7413.6261127600001</v>
+        <v>8172.7516339900003</v>
       </c>
       <c r="U38">
-        <v>8172.7516339900003</v>
+        <v>11310</v>
       </c>
       <c r="V38">
-        <v>11310</v>
-      </c>
-      <c r="W38">
         <v>12059</v>
       </c>
     </row>
-    <row r="39" spans="1:23">
+    <row r="39" spans="1:22">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -3507,34 +3393,31 @@
         <v>0.92434662242499999</v>
       </c>
       <c r="O39">
-        <v>0.61670153004299999</v>
+        <v>2.5613730904100001E-2</v>
       </c>
       <c r="P39">
-        <v>2.5613730904100001E-2</v>
+        <v>3820226</v>
       </c>
       <c r="Q39">
-        <v>3820226</v>
+        <v>14963</v>
       </c>
       <c r="R39">
         <v>14963</v>
       </c>
       <c r="S39">
-        <v>14963</v>
+        <v>2576.7314439900001</v>
       </c>
       <c r="T39">
-        <v>2576.7314439900001</v>
+        <v>2758.28592058</v>
       </c>
       <c r="U39">
-        <v>2758.28592058</v>
+        <v>3108</v>
       </c>
       <c r="V39">
-        <v>3108</v>
-      </c>
-      <c r="W39">
         <v>3297</v>
       </c>
     </row>
-    <row r="40" spans="1:23">
+    <row r="40" spans="1:22">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -3578,34 +3461,31 @@
         <v>0.88425800109599995</v>
       </c>
       <c r="O40">
-        <v>0.47656493695899999</v>
+        <v>2.0879359894399999E-2</v>
       </c>
       <c r="P40">
-        <v>2.0879359894399999E-2</v>
+        <v>4632709</v>
       </c>
       <c r="Q40">
-        <v>4632709</v>
+        <v>14576</v>
       </c>
       <c r="R40">
         <v>14576</v>
       </c>
       <c r="S40">
-        <v>14576</v>
+        <v>2590.84955257</v>
       </c>
       <c r="T40">
-        <v>2590.84955257</v>
+        <v>2630.7262918800002</v>
       </c>
       <c r="U40">
-        <v>2630.7262918800002</v>
+        <v>3071</v>
       </c>
       <c r="V40">
-        <v>3071</v>
-      </c>
-      <c r="W40">
         <v>3117</v>
       </c>
     </row>
-    <row r="41" spans="1:23">
+    <row r="41" spans="1:22">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -3649,34 +3529,31 @@
         <v>0.927737486399</v>
       </c>
       <c r="O41">
-        <v>0.45351313265499998</v>
+        <v>2.96749715916E-2</v>
       </c>
       <c r="P41">
-        <v>2.96749715916E-2</v>
+        <v>5370876</v>
       </c>
       <c r="Q41">
-        <v>5370876</v>
+        <v>250963</v>
       </c>
       <c r="R41">
-        <v>250963</v>
+        <v>309697</v>
       </c>
       <c r="S41">
-        <v>309697</v>
+        <v>29508.274725300002</v>
       </c>
       <c r="T41">
-        <v>29508.274725300002</v>
+        <v>31226.023255799999</v>
       </c>
       <c r="U41">
-        <v>31226.023255799999</v>
+        <v>64760</v>
       </c>
       <c r="V41">
-        <v>64760</v>
-      </c>
-      <c r="W41">
         <v>76899</v>
       </c>
     </row>
-    <row r="42" spans="1:23">
+    <row r="42" spans="1:22">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -3720,34 +3597,31 @@
         <v>0.90559616785599995</v>
       </c>
       <c r="O42">
-        <v>0.641940178694</v>
+        <v>2.26216487452E-2</v>
       </c>
       <c r="P42">
-        <v>2.26216487452E-2</v>
+        <v>3073371</v>
       </c>
       <c r="Q42">
-        <v>3073371</v>
+        <v>11633</v>
       </c>
       <c r="R42">
-        <v>11633</v>
+        <v>13657</v>
       </c>
       <c r="S42">
-        <v>13657</v>
+        <v>2768.25654923</v>
       </c>
       <c r="T42">
-        <v>2768.25654923</v>
+        <v>3061.1264940199999</v>
       </c>
       <c r="U42">
-        <v>3061.1264940199999</v>
+        <v>2966</v>
       </c>
       <c r="V42">
-        <v>2966</v>
-      </c>
-      <c r="W42">
         <v>3284</v>
       </c>
     </row>
-    <row r="43" spans="1:23">
+    <row r="43" spans="1:22">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -3791,34 +3665,31 @@
         <v>0.87228637488100003</v>
       </c>
       <c r="O43">
-        <v>0.40974641229499997</v>
+        <v>2.3213603264500001E-2</v>
       </c>
       <c r="P43">
-        <v>2.3213603264500001E-2</v>
+        <v>2163849</v>
       </c>
       <c r="Q43">
-        <v>2163849</v>
+        <v>29870</v>
       </c>
       <c r="R43">
-        <v>29870</v>
+        <v>30157</v>
       </c>
       <c r="S43">
-        <v>30157</v>
+        <v>4951.2791761999997</v>
       </c>
       <c r="T43">
-        <v>4951.2791761999997</v>
+        <v>5115.4822695000003</v>
       </c>
       <c r="U43">
-        <v>5115.4822695000003</v>
+        <v>6696</v>
       </c>
       <c r="V43">
-        <v>6696</v>
-      </c>
-      <c r="W43">
         <v>6744</v>
       </c>
     </row>
-    <row r="44" spans="1:23">
+    <row r="44" spans="1:22">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -3862,34 +3733,31 @@
         <v>0.90116866296499998</v>
       </c>
       <c r="O44">
-        <v>0.60075577400299995</v>
+        <v>2.4501339595400001E-2</v>
       </c>
       <c r="P44">
-        <v>2.4501339595400001E-2</v>
+        <v>3654347</v>
       </c>
       <c r="Q44">
-        <v>3654347</v>
+        <v>55261</v>
       </c>
       <c r="R44">
         <v>55261</v>
       </c>
       <c r="S44">
-        <v>55261</v>
+        <v>5381.8365242999998</v>
       </c>
       <c r="T44">
-        <v>5381.8365242999998</v>
+        <v>5446.12071535</v>
       </c>
       <c r="U44">
-        <v>5446.12071535</v>
+        <v>7999</v>
       </c>
       <c r="V44">
-        <v>7999</v>
-      </c>
-      <c r="W44">
         <v>8141</v>
       </c>
     </row>
-    <row r="45" spans="1:23">
+    <row r="45" spans="1:22">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -3933,34 +3801,31 @@
         <v>0.94896588876800003</v>
       </c>
       <c r="O45">
-        <v>0.30749447364600002</v>
+        <v>2.5587032423400002E-2</v>
       </c>
       <c r="P45">
-        <v>2.5587032423400002E-2</v>
+        <v>772209</v>
       </c>
       <c r="Q45">
-        <v>772209</v>
+        <v>30626</v>
       </c>
       <c r="R45">
         <v>30626</v>
       </c>
       <c r="S45">
-        <v>30626</v>
+        <v>3231</v>
       </c>
       <c r="T45">
         <v>3231</v>
       </c>
       <c r="U45">
-        <v>3231</v>
+        <v>4406</v>
       </c>
       <c r="V45">
         <v>4406</v>
       </c>
-      <c r="W45">
-        <v>4406</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23">
+    </row>
+    <row r="46" spans="1:22">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -4004,34 +3869,31 @@
         <v>0.929237432576</v>
       </c>
       <c r="O46">
-        <v>0.53149712008600003</v>
+        <v>2.1449494180999999E-2</v>
       </c>
       <c r="P46">
-        <v>2.1449494180999999E-2</v>
+        <v>2044711</v>
       </c>
       <c r="Q46">
-        <v>2044711</v>
+        <v>23852</v>
       </c>
       <c r="R46">
         <v>23852</v>
       </c>
       <c r="S46">
-        <v>23852</v>
+        <v>2594.77030457</v>
       </c>
       <c r="T46">
-        <v>2594.77030457</v>
+        <v>2604.72738854</v>
       </c>
       <c r="U46">
-        <v>2604.72738854</v>
+        <v>3172</v>
       </c>
       <c r="V46">
-        <v>3172</v>
-      </c>
-      <c r="W46">
         <v>3178</v>
       </c>
     </row>
-    <row r="47" spans="1:23">
+    <row r="47" spans="1:22">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -4075,34 +3937,31 @@
         <v>0.95396739478399994</v>
       </c>
       <c r="O47">
-        <v>0.41521372301199999</v>
+        <v>1.3429964897400001E-2</v>
       </c>
       <c r="P47">
-        <v>1.3429964897400001E-2</v>
+        <v>1030878</v>
       </c>
       <c r="Q47">
-        <v>1030878</v>
+        <v>33870</v>
       </c>
       <c r="R47">
         <v>33870</v>
       </c>
       <c r="S47">
-        <v>33870</v>
+        <v>4858.38679245</v>
       </c>
       <c r="T47">
-        <v>4858.38679245</v>
+        <v>5313.8041237099997</v>
       </c>
       <c r="U47">
-        <v>5313.8041237099997</v>
+        <v>6692</v>
       </c>
       <c r="V47">
-        <v>6692</v>
-      </c>
-      <c r="W47">
         <v>7397</v>
       </c>
     </row>
-    <row r="48" spans="1:23">
+    <row r="48" spans="1:22">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -4146,34 +4005,31 @@
         <v>0.90489337016000004</v>
       </c>
       <c r="O48">
-        <v>0.40168755159000002</v>
+        <v>1.5071229269299999E-2</v>
       </c>
       <c r="P48">
-        <v>1.5071229269299999E-2</v>
+        <v>2384839</v>
       </c>
       <c r="Q48">
-        <v>2384839</v>
+        <v>26708</v>
       </c>
       <c r="R48">
-        <v>26708</v>
+        <v>34689</v>
       </c>
       <c r="S48">
-        <v>34689</v>
+        <v>5516.1550925900001</v>
       </c>
       <c r="T48">
-        <v>5516.1550925900001</v>
+        <v>5977.0401002500003</v>
       </c>
       <c r="U48">
-        <v>5977.0401002500003</v>
+        <v>7866</v>
       </c>
       <c r="V48">
-        <v>7866</v>
-      </c>
-      <c r="W48">
         <v>8694</v>
       </c>
     </row>
-    <row r="49" spans="1:23">
+    <row r="49" spans="1:22">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -4217,34 +4073,31 @@
         <v>0.92057691392499996</v>
       </c>
       <c r="O49">
-        <v>0.49053830240599999</v>
+        <v>1.95720974468E-2</v>
       </c>
       <c r="P49">
-        <v>1.95720974468E-2</v>
+        <v>2899774</v>
       </c>
       <c r="Q49">
-        <v>2899774</v>
+        <v>13565</v>
       </c>
       <c r="R49">
         <v>13565</v>
       </c>
       <c r="S49">
-        <v>13565</v>
+        <v>2362.9779951099999</v>
       </c>
       <c r="T49">
-        <v>2362.9779951099999</v>
+        <v>2442.9435551800002</v>
       </c>
       <c r="U49">
-        <v>2442.9435551800002</v>
+        <v>2818</v>
       </c>
       <c r="V49">
-        <v>2818</v>
-      </c>
-      <c r="W49">
         <v>2880</v>
       </c>
     </row>
-    <row r="50" spans="1:23">
+    <row r="50" spans="1:22">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -4288,34 +4141,31 @@
         <v>0.87093150923700002</v>
       </c>
       <c r="O50">
-        <v>0.42153996433000002</v>
+        <v>1.27434576777E-2</v>
       </c>
       <c r="P50">
-        <v>1.27434576777E-2</v>
+        <v>3086679</v>
       </c>
       <c r="Q50">
-        <v>3086679</v>
+        <v>32856</v>
       </c>
       <c r="R50">
         <v>32856</v>
       </c>
       <c r="S50">
-        <v>32856</v>
+        <v>6872.0244988900004</v>
       </c>
       <c r="T50">
-        <v>6872.0244988900004</v>
+        <v>7419.9014423099998</v>
       </c>
       <c r="U50">
-        <v>7419.9014423099998</v>
+        <v>8960</v>
       </c>
       <c r="V50">
-        <v>8960</v>
-      </c>
-      <c r="W50">
         <v>9351</v>
       </c>
     </row>
-    <row r="51" spans="1:23">
+    <row r="51" spans="1:22">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -4359,34 +4209,31 @@
         <v>0.93974835331899997</v>
       </c>
       <c r="O51">
-        <v>0.36916958298800001</v>
+        <v>1.9209260571699999E-2</v>
       </c>
       <c r="P51">
-        <v>1.9209260571699999E-2</v>
+        <v>899992</v>
       </c>
       <c r="Q51">
-        <v>899992</v>
+        <v>25616</v>
       </c>
       <c r="R51">
         <v>25616</v>
       </c>
       <c r="S51">
-        <v>25616</v>
+        <v>4560.3654822300005</v>
       </c>
       <c r="T51">
-        <v>4560.3654822300005</v>
+        <v>4972.3314917099997</v>
       </c>
       <c r="U51">
-        <v>4972.3314917099997</v>
+        <v>6965</v>
       </c>
       <c r="V51">
-        <v>6965</v>
-      </c>
-      <c r="W51">
         <v>8370</v>
       </c>
     </row>
-    <row r="52" spans="1:23">
+    <row r="52" spans="1:22">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -4430,34 +4277,31 @@
         <v>0.94857047945399997</v>
       </c>
       <c r="O52">
-        <v>0.35826100784600001</v>
+        <v>1.7743657404899998E-2</v>
       </c>
       <c r="P52">
-        <v>1.7743657404899998E-2</v>
+        <v>1547302</v>
       </c>
       <c r="Q52">
-        <v>1547302</v>
+        <v>9790</v>
       </c>
       <c r="R52">
         <v>9790</v>
       </c>
       <c r="S52">
-        <v>9790</v>
+        <v>2617.4991539799998</v>
       </c>
       <c r="T52">
-        <v>2617.4991539799998</v>
+        <v>2658.5945017200002</v>
       </c>
       <c r="U52">
-        <v>2658.5945017200002</v>
+        <v>3167</v>
       </c>
       <c r="V52">
-        <v>3167</v>
-      </c>
-      <c r="W52">
         <v>3211</v>
       </c>
     </row>
-    <row r="53" spans="1:23">
+    <row r="53" spans="1:22">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -4501,34 +4345,31 @@
         <v>0.94925102002600004</v>
       </c>
       <c r="O53">
-        <v>0.46080462608700001</v>
+        <v>9.4766529763199991E-3</v>
       </c>
       <c r="P53">
-        <v>9.4766529763199991E-3</v>
+        <v>1248498</v>
       </c>
       <c r="Q53">
-        <v>1248498</v>
+        <v>143658</v>
       </c>
       <c r="R53">
         <v>143658</v>
       </c>
       <c r="S53">
-        <v>143658</v>
+        <v>21138.779661</v>
       </c>
       <c r="T53">
-        <v>21138.779661</v>
+        <v>27744.400000000001</v>
       </c>
       <c r="U53">
-        <v>27744.400000000001</v>
+        <v>42501</v>
       </c>
       <c r="V53">
-        <v>42501</v>
-      </c>
-      <c r="W53">
         <v>48609</v>
       </c>
     </row>
-    <row r="54" spans="1:23">
+    <row r="54" spans="1:22">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -4572,34 +4413,31 @@
         <v>0.82367559783300004</v>
       </c>
       <c r="O54">
-        <v>0.428313262995</v>
+        <v>3.4668486122700001E-2</v>
       </c>
       <c r="P54">
-        <v>3.4668486122700001E-2</v>
+        <v>5131655</v>
       </c>
       <c r="Q54">
-        <v>5131655</v>
+        <v>63319</v>
       </c>
       <c r="R54">
         <v>63319</v>
       </c>
       <c r="S54">
-        <v>63319</v>
+        <v>7094.1147994499997</v>
       </c>
       <c r="T54">
-        <v>7094.1147994499997</v>
+        <v>7670.6352765299998</v>
       </c>
       <c r="U54">
-        <v>7670.6352765299998</v>
+        <v>11085</v>
       </c>
       <c r="V54">
-        <v>11085</v>
-      </c>
-      <c r="W54">
         <v>11754</v>
       </c>
     </row>
-    <row r="55" spans="1:23">
+    <row r="55" spans="1:22">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -4643,34 +4481,31 @@
         <v>0.95425970425999995</v>
       </c>
       <c r="O55">
-        <v>0.37133265381000002</v>
+        <v>1.9266796353499999E-2</v>
       </c>
       <c r="P55">
-        <v>1.9266796353499999E-2</v>
+        <v>888888</v>
       </c>
       <c r="Q55">
-        <v>888888</v>
+        <v>48728</v>
       </c>
       <c r="R55">
         <v>48728</v>
       </c>
       <c r="S55">
-        <v>48728</v>
+        <v>5387.0181818199999</v>
       </c>
       <c r="T55">
-        <v>5387.0181818199999</v>
+        <v>5486.9629629600004</v>
       </c>
       <c r="U55">
-        <v>5486.9629629600004</v>
+        <v>8576</v>
       </c>
       <c r="V55">
         <v>8576</v>
       </c>
-      <c r="W55">
-        <v>8576</v>
-      </c>
-    </row>
-    <row r="56" spans="1:23">
+    </row>
+    <row r="56" spans="1:22">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -4714,34 +4549,31 @@
         <v>0.90259746188300005</v>
       </c>
       <c r="O56">
-        <v>0.363361707295</v>
+        <v>2.1567572142500002E-2</v>
       </c>
       <c r="P56">
-        <v>2.1567572142500002E-2</v>
+        <v>1095300</v>
       </c>
       <c r="Q56">
-        <v>1095300</v>
+        <v>72086</v>
       </c>
       <c r="R56">
         <v>72086</v>
       </c>
       <c r="S56">
-        <v>72086</v>
+        <v>10236.009345799999</v>
       </c>
       <c r="T56">
-        <v>10236.009345799999</v>
+        <v>10531.730769199999</v>
       </c>
       <c r="U56">
-        <v>10531.730769199999</v>
+        <v>20151</v>
       </c>
       <c r="V56">
         <v>20151</v>
       </c>
-      <c r="W56">
-        <v>20151</v>
-      </c>
-    </row>
-    <row r="57" spans="1:23">
+    </row>
+    <row r="57" spans="1:22">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -4785,34 +4617,31 @@
         <v>0.84112431892299999</v>
       </c>
       <c r="O57">
-        <v>0.600770143039</v>
+        <v>1.48216730561E-2</v>
       </c>
       <c r="P57">
-        <v>1.48216730561E-2</v>
+        <v>6556894</v>
       </c>
       <c r="Q57">
-        <v>6556894</v>
+        <v>47199</v>
       </c>
       <c r="R57">
         <v>47199</v>
       </c>
       <c r="S57">
-        <v>47199</v>
+        <v>6396.0243902399998</v>
       </c>
       <c r="T57">
-        <v>6396.0243902399998</v>
+        <v>7058.0129171199997</v>
       </c>
       <c r="U57">
-        <v>7058.0129171199997</v>
+        <v>9012</v>
       </c>
       <c r="V57">
-        <v>9012</v>
-      </c>
-      <c r="W57">
         <v>9888</v>
       </c>
     </row>
-    <row r="58" spans="1:23">
+    <row r="58" spans="1:22">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -4856,34 +4685,31 @@
         <v>0.91867179757499995</v>
       </c>
       <c r="O58">
-        <v>0.42068433507500003</v>
+        <v>1.9480629570300001E-2</v>
       </c>
       <c r="P58">
-        <v>1.9480629570300001E-2</v>
+        <v>3663809</v>
       </c>
       <c r="Q58">
-        <v>3663809</v>
+        <v>170187</v>
       </c>
       <c r="R58">
         <v>170187</v>
       </c>
       <c r="S58">
-        <v>170187</v>
+        <v>11093.360606099999</v>
       </c>
       <c r="T58">
-        <v>11093.360606099999</v>
+        <v>12590.408934700001</v>
       </c>
       <c r="U58">
-        <v>12590.408934700001</v>
+        <v>19929</v>
       </c>
       <c r="V58">
-        <v>19929</v>
-      </c>
-      <c r="W58">
         <v>24275</v>
       </c>
     </row>
-    <row r="59" spans="1:23">
+    <row r="59" spans="1:22">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -4927,34 +4753,31 @@
         <v>0.89059197803300005</v>
       </c>
       <c r="O59">
-        <v>0.58732212729599997</v>
+        <v>2.89735133448E-2</v>
       </c>
       <c r="P59">
-        <v>2.89735133448E-2</v>
+        <v>6818851</v>
       </c>
       <c r="Q59">
-        <v>6818851</v>
+        <v>183583</v>
       </c>
       <c r="R59">
         <v>183583</v>
       </c>
       <c r="S59">
-        <v>183583</v>
+        <v>9630.3516949200002</v>
       </c>
       <c r="T59">
-        <v>9630.3516949200002</v>
+        <v>9839.6118326100004</v>
       </c>
       <c r="U59">
-        <v>9839.6118326100004</v>
+        <v>22103</v>
       </c>
       <c r="V59">
-        <v>22103</v>
-      </c>
-      <c r="W59">
         <v>22220</v>
       </c>
     </row>
-    <row r="60" spans="1:23">
+    <row r="60" spans="1:22">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -4998,34 +4821,31 @@
         <v>0.88405447876400001</v>
       </c>
       <c r="O60">
-        <v>0.41435703116799999</v>
+        <v>3.0270736756500001E-2</v>
       </c>
       <c r="P60">
-        <v>3.0270736756500001E-2</v>
+        <v>2523185</v>
       </c>
       <c r="Q60">
-        <v>2523185</v>
+        <v>60467</v>
       </c>
       <c r="R60">
         <v>60467</v>
       </c>
       <c r="S60">
-        <v>60467</v>
+        <v>2999.9346016600002</v>
       </c>
       <c r="T60">
-        <v>2999.9346016600002</v>
+        <v>3088.3537331699999</v>
       </c>
       <c r="U60">
-        <v>3088.3537331699999</v>
+        <v>3481</v>
       </c>
       <c r="V60">
-        <v>3481</v>
-      </c>
-      <c r="W60">
         <v>3510</v>
       </c>
     </row>
-    <row r="61" spans="1:23">
+    <row r="61" spans="1:22">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -5069,34 +4889,31 @@
         <v>0.90204267815700001</v>
       </c>
       <c r="O61">
-        <v>0.55914385824699997</v>
+        <v>8.0101606262600003E-2</v>
       </c>
       <c r="P61">
-        <v>8.0101606262600003E-2</v>
+        <v>2582492</v>
       </c>
       <c r="Q61">
-        <v>2582492</v>
+        <v>215276</v>
       </c>
       <c r="R61">
         <v>215276</v>
       </c>
       <c r="S61">
-        <v>215276</v>
+        <v>12717.8423645</v>
       </c>
       <c r="T61">
-        <v>12717.8423645</v>
+        <v>13663.978836</v>
       </c>
       <c r="U61">
-        <v>13663.978836</v>
+        <v>81540</v>
       </c>
       <c r="V61">
-        <v>81540</v>
-      </c>
-      <c r="W61">
         <v>93032</v>
       </c>
     </row>
-    <row r="62" spans="1:23">
+    <row r="62" spans="1:22">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -5140,34 +4957,31 @@
         <v>0.91270000281800001</v>
       </c>
       <c r="O62">
-        <v>0.40112991732800002</v>
+        <v>1.87386093351E-2</v>
       </c>
       <c r="P62">
-        <v>1.87386093351E-2</v>
+        <v>2590401</v>
       </c>
       <c r="Q62">
-        <v>2590401</v>
+        <v>17793</v>
       </c>
       <c r="R62">
         <v>17793</v>
       </c>
       <c r="S62">
-        <v>17793</v>
+        <v>4191.1019417500002</v>
       </c>
       <c r="T62">
-        <v>4191.1019417500002</v>
+        <v>4405.4438775500003</v>
       </c>
       <c r="U62">
-        <v>4405.4438775500003</v>
+        <v>4882</v>
       </c>
       <c r="V62">
-        <v>4882</v>
-      </c>
-      <c r="W62">
         <v>4993</v>
       </c>
     </row>
-    <row r="63" spans="1:23">
+    <row r="63" spans="1:22">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -5211,34 +5025,31 @@
         <v>0.935920816451</v>
       </c>
       <c r="O63">
-        <v>0.616665567139</v>
+        <v>1.2851757007E-2</v>
       </c>
       <c r="P63">
-        <v>1.2851757007E-2</v>
+        <v>3204504</v>
       </c>
       <c r="Q63">
-        <v>3204504</v>
+        <v>52440</v>
       </c>
       <c r="R63">
-        <v>52440</v>
+        <v>57913</v>
       </c>
       <c r="S63">
-        <v>57913</v>
+        <v>7352.5126436800001</v>
       </c>
       <c r="T63">
-        <v>7352.5126436800001</v>
+        <v>8779.4630137000004</v>
       </c>
       <c r="U63">
-        <v>8779.4630137000004</v>
+        <v>14607</v>
       </c>
       <c r="V63">
-        <v>14607</v>
-      </c>
-      <c r="W63">
         <v>16305</v>
       </c>
     </row>
-    <row r="64" spans="1:23">
+    <row r="64" spans="1:22">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -5282,34 +5093,31 @@
         <v>0.88866408294200006</v>
       </c>
       <c r="O64">
-        <v>0.42228794678499998</v>
+        <v>1.7145893920700001E-2</v>
       </c>
       <c r="P64">
-        <v>1.7145893920700001E-2</v>
+        <v>3598165</v>
       </c>
       <c r="Q64">
-        <v>3598165</v>
+        <v>121245</v>
       </c>
       <c r="R64">
         <v>121245</v>
       </c>
       <c r="S64">
-        <v>121245</v>
+        <v>29487.745901599999</v>
       </c>
       <c r="T64">
-        <v>29487.745901599999</v>
+        <v>32710.590909099999</v>
       </c>
       <c r="U64">
-        <v>32710.590909099999</v>
+        <v>43371</v>
       </c>
       <c r="V64">
-        <v>43371</v>
-      </c>
-      <c r="W64">
         <v>48384</v>
       </c>
     </row>
-    <row r="65" spans="1:23">
+    <row r="65" spans="1:22">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -5353,34 +5161,31 @@
         <v>0.88337850048900002</v>
       </c>
       <c r="O65">
-        <v>0.50339937105499999</v>
+        <v>1.6498957450100001E-2</v>
       </c>
       <c r="P65">
-        <v>1.6498957450100001E-2</v>
+        <v>2393701</v>
       </c>
       <c r="Q65">
-        <v>2393701</v>
+        <v>171045</v>
       </c>
       <c r="R65">
-        <v>171045</v>
+        <v>202111</v>
       </c>
       <c r="S65">
-        <v>202111</v>
+        <v>28837.722891599999</v>
       </c>
       <c r="T65">
-        <v>28837.722891599999</v>
+        <v>31916.013333300001</v>
       </c>
       <c r="U65">
-        <v>31916.013333300001</v>
+        <v>62417</v>
       </c>
       <c r="V65">
-        <v>62417</v>
-      </c>
-      <c r="W65">
         <v>64334</v>
       </c>
     </row>
-    <row r="66" spans="1:23">
+    <row r="66" spans="1:22">
       <c r="A66" s="1" t="s">
         <v>64</v>
       </c>
@@ -5424,34 +5229,31 @@
         <v>0.85586859986099995</v>
       </c>
       <c r="O66">
-        <v>0.45762470232500002</v>
+        <v>4.0974862630800003E-2</v>
       </c>
       <c r="P66">
-        <v>4.0974862630800003E-2</v>
+        <v>4672750</v>
       </c>
       <c r="Q66">
-        <v>4672750</v>
+        <v>87705</v>
       </c>
       <c r="R66">
         <v>87705</v>
       </c>
       <c r="S66">
-        <v>87705</v>
+        <v>7462.6597444099998</v>
       </c>
       <c r="T66">
-        <v>7462.6597444099998</v>
+        <v>7762.0431893699997</v>
       </c>
       <c r="U66">
-        <v>7762.0431893699997</v>
+        <v>19396</v>
       </c>
       <c r="V66">
-        <v>19396</v>
-      </c>
-      <c r="W66">
         <v>20140</v>
       </c>
     </row>
-    <row r="67" spans="1:23">
+    <row r="67" spans="1:22">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -5495,34 +5297,31 @@
         <v>0.95637964977599998</v>
       </c>
       <c r="O67">
-        <v>0.44516448047000001</v>
+        <v>8.3145272488399993E-3</v>
       </c>
       <c r="P67">
-        <v>8.3145272488399993E-3</v>
+        <v>1246001</v>
       </c>
       <c r="Q67">
-        <v>1246001</v>
+        <v>126814</v>
       </c>
       <c r="R67">
         <v>126814</v>
       </c>
       <c r="S67">
-        <v>126814</v>
+        <v>18054.652173900002</v>
       </c>
       <c r="T67">
-        <v>18054.652173900002</v>
+        <v>19468.765625</v>
       </c>
       <c r="U67">
-        <v>19468.765625</v>
+        <v>33498</v>
       </c>
       <c r="V67">
         <v>33498</v>
       </c>
-      <c r="W67">
-        <v>33498</v>
-      </c>
-    </row>
-    <row r="68" spans="1:23">
+    </row>
+    <row r="68" spans="1:22">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -5566,34 +5365,31 @@
         <v>0.94118148770499999</v>
       </c>
       <c r="O68">
-        <v>0.54104633180999995</v>
+        <v>1.5354788097199999E-2</v>
       </c>
       <c r="P68">
-        <v>1.5354788097199999E-2</v>
+        <v>1735236</v>
       </c>
       <c r="Q68">
-        <v>1735236</v>
+        <v>105405</v>
       </c>
       <c r="R68">
         <v>105405</v>
       </c>
       <c r="S68">
-        <v>105405</v>
+        <v>13635.637795299999</v>
       </c>
       <c r="T68">
-        <v>13635.637795299999</v>
+        <v>19068.527472500002</v>
       </c>
       <c r="U68">
-        <v>19068.527472500002</v>
+        <v>26219</v>
       </c>
       <c r="V68">
-        <v>26219</v>
-      </c>
-      <c r="W68">
         <v>38177</v>
       </c>
     </row>
-    <row r="69" spans="1:23">
+    <row r="69" spans="1:22">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -5637,34 +5433,31 @@
         <v>0.91317095964499995</v>
       </c>
       <c r="O69">
-        <v>0.37696486999399997</v>
+        <v>1.94068260892E-2</v>
       </c>
       <c r="P69">
-        <v>1.94068260892E-2</v>
+        <v>2709347</v>
       </c>
       <c r="Q69">
-        <v>2709347</v>
+        <v>16190</v>
       </c>
       <c r="R69">
-        <v>16190</v>
+        <v>16315</v>
       </c>
       <c r="S69">
-        <v>16315</v>
+        <v>3908.7546897500001</v>
       </c>
       <c r="T69">
-        <v>3908.7546897500001</v>
+        <v>4092.66918429</v>
       </c>
       <c r="U69">
-        <v>4092.66918429</v>
+        <v>4998</v>
       </c>
       <c r="V69">
-        <v>4998</v>
-      </c>
-      <c r="W69">
         <v>5083</v>
       </c>
     </row>
-    <row r="70" spans="1:23">
+    <row r="70" spans="1:22">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -5708,34 +5501,31 @@
         <v>0.91872560740599996</v>
       </c>
       <c r="O70">
-        <v>0.548581516012</v>
+        <v>3.0846721471599999E-2</v>
       </c>
       <c r="P70">
-        <v>3.0846721471599999E-2</v>
+        <v>1834317</v>
       </c>
       <c r="Q70">
-        <v>1834317</v>
+        <v>13066</v>
       </c>
       <c r="R70">
         <v>13066</v>
       </c>
       <c r="S70">
-        <v>13066</v>
+        <v>2939.4983974400002</v>
       </c>
       <c r="T70">
-        <v>2939.4983974400002</v>
+        <v>2972.96110211</v>
       </c>
       <c r="U70">
-        <v>2972.96110211</v>
+        <v>3586</v>
       </c>
       <c r="V70">
-        <v>3586</v>
-      </c>
-      <c r="W70">
         <v>3631</v>
       </c>
     </row>
-    <row r="71" spans="1:23">
+    <row r="71" spans="1:22">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -5779,34 +5569,31 @@
         <v>0.94556896576600002</v>
       </c>
       <c r="O71">
-        <v>0.454944510222</v>
+        <v>1.7025302859500002E-2</v>
       </c>
       <c r="P71">
-        <v>1.7025302859500002E-2</v>
+        <v>2009497</v>
       </c>
       <c r="Q71">
-        <v>2009497</v>
+        <v>73982</v>
       </c>
       <c r="R71">
         <v>73982</v>
       </c>
       <c r="S71">
-        <v>73982</v>
+        <v>9010.2645739899999</v>
       </c>
       <c r="T71">
-        <v>9010.2645739899999</v>
+        <v>9850.4754902000004</v>
       </c>
       <c r="U71">
-        <v>9850.4754902000004</v>
+        <v>19759</v>
       </c>
       <c r="V71">
-        <v>19759</v>
-      </c>
-      <c r="W71">
         <v>20597</v>
       </c>
     </row>
-    <row r="72" spans="1:23">
+    <row r="72" spans="1:22">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -5850,34 +5637,31 @@
         <v>0.94330568967299999</v>
       </c>
       <c r="O72">
-        <v>0.54824494024799997</v>
+        <v>3.5233001702199999E-2</v>
       </c>
       <c r="P72">
-        <v>3.5233001702199999E-2</v>
+        <v>3359420</v>
       </c>
       <c r="Q72">
-        <v>3359420</v>
+        <v>175702</v>
       </c>
       <c r="R72">
         <v>175702</v>
       </c>
       <c r="S72">
-        <v>175702</v>
+        <v>21258.607594900001</v>
       </c>
       <c r="T72">
-        <v>21258.607594900001</v>
+        <v>22853.197278899999</v>
       </c>
       <c r="U72">
-        <v>22853.197278899999</v>
+        <v>58348</v>
       </c>
       <c r="V72">
-        <v>58348</v>
-      </c>
-      <c r="W72">
         <v>66549</v>
       </c>
     </row>
-    <row r="73" spans="1:23">
+    <row r="73" spans="1:22">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -5921,34 +5705,31 @@
         <v>0.917516562285</v>
       </c>
       <c r="O73">
-        <v>0.50289779364300002</v>
+        <v>2.4469531554100001E-2</v>
       </c>
       <c r="P73">
-        <v>2.4469531554100001E-2</v>
+        <v>1381150</v>
       </c>
       <c r="Q73">
-        <v>1381150</v>
+        <v>47790</v>
       </c>
       <c r="R73">
         <v>47790</v>
       </c>
       <c r="S73">
-        <v>47790</v>
+        <v>4656.3851351399999</v>
       </c>
       <c r="T73">
-        <v>4656.3851351399999</v>
+        <v>5271.5648854999999</v>
       </c>
       <c r="U73">
-        <v>5271.5648854999999</v>
+        <v>8131</v>
       </c>
       <c r="V73">
-        <v>8131</v>
-      </c>
-      <c r="W73">
         <v>9758</v>
       </c>
     </row>
-    <row r="74" spans="1:23">
+    <row r="74" spans="1:22">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -5992,34 +5773,31 @@
         <v>0.92718183892799999</v>
       </c>
       <c r="O74">
-        <v>0.35471735041199998</v>
+        <v>2.11142214406E-2</v>
       </c>
       <c r="P74">
-        <v>2.11142214406E-2</v>
+        <v>2300525</v>
       </c>
       <c r="Q74">
-        <v>2300525</v>
+        <v>16126</v>
       </c>
       <c r="R74">
         <v>16126</v>
       </c>
       <c r="S74">
-        <v>16126</v>
+        <v>3098.6859838300002</v>
       </c>
       <c r="T74">
-        <v>3098.6859838300002</v>
+        <v>3235.6188466899998</v>
       </c>
       <c r="U74">
-        <v>3235.6188466899998</v>
+        <v>3733</v>
       </c>
       <c r="V74">
-        <v>3733</v>
-      </c>
-      <c r="W74">
         <v>3909</v>
       </c>
     </row>
-    <row r="75" spans="1:23">
+    <row r="75" spans="1:22">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -6063,34 +5841,31 @@
         <v>0.92097304736899999</v>
       </c>
       <c r="O75">
-        <v>0.63486043802900005</v>
+        <v>2.1431666149600001E-2</v>
       </c>
       <c r="P75">
-        <v>2.1431666149600001E-2</v>
+        <v>3605251</v>
       </c>
       <c r="Q75">
-        <v>3605251</v>
+        <v>139656</v>
       </c>
       <c r="R75">
         <v>139656</v>
       </c>
       <c r="S75">
-        <v>139656</v>
+        <v>11898.0231023</v>
       </c>
       <c r="T75">
-        <v>11898.0231023</v>
+        <v>12138.8922559</v>
       </c>
       <c r="U75">
-        <v>12138.8922559</v>
+        <v>20670</v>
       </c>
       <c r="V75">
-        <v>20670</v>
-      </c>
-      <c r="W75">
         <v>20702</v>
       </c>
     </row>
-    <row r="76" spans="1:23">
+    <row r="76" spans="1:22">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -6134,34 +5909,31 @@
         <v>0.87490070528099995</v>
       </c>
       <c r="O76">
-        <v>0.467403504824</v>
+        <v>1.9061285317499999E-2</v>
       </c>
       <c r="P76">
-        <v>1.9061285317499999E-2</v>
+        <v>3858463</v>
       </c>
       <c r="Q76">
-        <v>3858463</v>
+        <v>23804</v>
       </c>
       <c r="R76">
         <v>23804</v>
       </c>
       <c r="S76">
-        <v>23804</v>
+        <v>2211.9575688099999</v>
       </c>
       <c r="T76">
-        <v>2211.9575688099999</v>
+        <v>2318.7878605800001</v>
       </c>
       <c r="U76">
-        <v>2318.7878605800001</v>
+        <v>2677</v>
       </c>
       <c r="V76">
-        <v>2677</v>
-      </c>
-      <c r="W76">
         <v>2767</v>
       </c>
     </row>
-    <row r="77" spans="1:23">
+    <row r="77" spans="1:22">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -6205,34 +5977,31 @@
         <v>0.93993554261800005</v>
       </c>
       <c r="O77">
-        <v>0.53987356489600002</v>
+        <v>1.9208380762900001E-2</v>
       </c>
       <c r="P77">
-        <v>1.9208380762900001E-2</v>
+        <v>1437539</v>
       </c>
       <c r="Q77">
-        <v>1437539</v>
+        <v>47947</v>
       </c>
       <c r="R77">
-        <v>47947</v>
+        <v>58904</v>
       </c>
       <c r="S77">
-        <v>58904</v>
+        <v>4000.1089385499999</v>
       </c>
       <c r="T77">
-        <v>4000.1089385499999</v>
+        <v>4744.3531353099997</v>
       </c>
       <c r="U77">
-        <v>4744.3531353099997</v>
+        <v>4878</v>
       </c>
       <c r="V77">
-        <v>4878</v>
-      </c>
-      <c r="W77">
         <v>6969</v>
       </c>
     </row>
-    <row r="78" spans="1:23">
+    <row r="78" spans="1:22">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -6276,34 +6045,31 @@
         <v>0.916012306921</v>
       </c>
       <c r="O78">
-        <v>0.63365888288299999</v>
+        <v>1.7486109183899999E-2</v>
       </c>
       <c r="P78">
-        <v>1.7486109183899999E-2</v>
+        <v>3831990</v>
       </c>
       <c r="Q78">
-        <v>3831990</v>
+        <v>32481</v>
       </c>
       <c r="R78">
         <v>32481</v>
       </c>
       <c r="S78">
-        <v>32481</v>
+        <v>4003.62591432</v>
       </c>
       <c r="T78">
-        <v>4003.62591432</v>
+        <v>4234.2430939200003</v>
       </c>
       <c r="U78">
-        <v>4234.2430939200003</v>
+        <v>5741</v>
       </c>
       <c r="V78">
-        <v>5741</v>
-      </c>
-      <c r="W78">
         <v>6004</v>
       </c>
     </row>
-    <row r="79" spans="1:23">
+    <row r="79" spans="1:22">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -6347,34 +6113,31 @@
         <v>0.914262675247</v>
       </c>
       <c r="O79">
-        <v>0.59980964609599996</v>
+        <v>3.2118033939700003E-2</v>
       </c>
       <c r="P79">
-        <v>3.2118033939700003E-2</v>
+        <v>3916334</v>
       </c>
       <c r="Q79">
-        <v>3916334</v>
+        <v>57390</v>
       </c>
       <c r="R79">
         <v>57390</v>
       </c>
       <c r="S79">
-        <v>57390</v>
+        <v>6398.4705882400003</v>
       </c>
       <c r="T79">
-        <v>6398.4705882400003</v>
+        <v>6931.5646017700001</v>
       </c>
       <c r="U79">
-        <v>6931.5646017700001</v>
+        <v>11827</v>
       </c>
       <c r="V79">
-        <v>11827</v>
-      </c>
-      <c r="W79">
         <v>11946</v>
       </c>
     </row>
-    <row r="80" spans="1:23">
+    <row r="80" spans="1:22">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -6418,34 +6181,31 @@
         <v>0.83031599626499997</v>
       </c>
       <c r="O80">
-        <v>0.44711157065500001</v>
+        <v>3.1205465943199999E-2</v>
       </c>
       <c r="P80">
-        <v>3.1205465943199999E-2</v>
+        <v>4632175</v>
       </c>
       <c r="Q80">
-        <v>4632175</v>
+        <v>45716</v>
       </c>
       <c r="R80">
         <v>45716</v>
       </c>
       <c r="S80">
-        <v>45716</v>
+        <v>6082.4494086699997</v>
       </c>
       <c r="T80">
-        <v>6082.4494086699997</v>
+        <v>6460.4951185500004</v>
       </c>
       <c r="U80">
-        <v>6460.4951185500004</v>
+        <v>10977</v>
       </c>
       <c r="V80">
-        <v>10977</v>
-      </c>
-      <c r="W80">
         <v>11579</v>
       </c>
     </row>
-    <row r="81" spans="1:23">
+    <row r="81" spans="1:22">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -6489,34 +6249,31 @@
         <v>0.90737881471699999</v>
       </c>
       <c r="O81">
-        <v>0.485126221528</v>
+        <v>2.1781066411099999E-2</v>
       </c>
       <c r="P81">
-        <v>2.1781066411099999E-2</v>
+        <v>2613333</v>
       </c>
       <c r="Q81">
-        <v>2613333</v>
+        <v>32749</v>
       </c>
       <c r="R81">
         <v>32749</v>
       </c>
       <c r="S81">
-        <v>32749</v>
+        <v>7340.5140449399996</v>
       </c>
       <c r="T81">
-        <v>7340.5140449399996</v>
+        <v>7574.8782608700003</v>
       </c>
       <c r="U81">
-        <v>7574.8782608700003</v>
+        <v>11047</v>
       </c>
       <c r="V81">
-        <v>11047</v>
-      </c>
-      <c r="W81">
         <v>11388</v>
       </c>
     </row>
-    <row r="82" spans="1:23">
+    <row r="82" spans="1:22">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -6560,34 +6317,31 @@
         <v>0.91892298430599995</v>
       </c>
       <c r="O82">
-        <v>0.54914516747599995</v>
+        <v>2.8556419886800001E-2</v>
       </c>
       <c r="P82">
-        <v>2.8556419886800001E-2</v>
+        <v>2971693</v>
       </c>
       <c r="Q82">
-        <v>2971693</v>
+        <v>129573</v>
       </c>
       <c r="R82">
-        <v>129573</v>
+        <v>162795</v>
       </c>
       <c r="S82">
-        <v>162795</v>
+        <v>13622.766055</v>
       </c>
       <c r="T82">
-        <v>13622.766055</v>
+        <v>15161.6989796</v>
       </c>
       <c r="U82">
-        <v>15161.6989796</v>
+        <v>61701</v>
       </c>
       <c r="V82">
-        <v>61701</v>
-      </c>
-      <c r="W82">
         <v>71658</v>
       </c>
     </row>
-    <row r="83" spans="1:23">
+    <row r="83" spans="1:22">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -6631,34 +6385,31 @@
         <v>0.87279459128900005</v>
       </c>
       <c r="O83">
-        <v>0.42462792219500001</v>
+        <v>2.0015698111900002E-2</v>
       </c>
       <c r="P83">
-        <v>2.0015698111900002E-2</v>
+        <v>3312878</v>
       </c>
       <c r="Q83">
-        <v>3312878</v>
+        <v>70636</v>
       </c>
       <c r="R83">
-        <v>70636</v>
+        <v>76716</v>
       </c>
       <c r="S83">
-        <v>76716</v>
+        <v>7556.9086758000003</v>
       </c>
       <c r="T83">
-        <v>7556.9086758000003</v>
+        <v>8220.5409429299998</v>
       </c>
       <c r="U83">
-        <v>8220.5409429299998</v>
+        <v>15460</v>
       </c>
       <c r="V83">
-        <v>15460</v>
-      </c>
-      <c r="W83">
         <v>16076</v>
       </c>
     </row>
-    <row r="84" spans="1:23">
+    <row r="84" spans="1:22">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -6702,34 +6453,31 @@
         <v>0.95586159086800004</v>
       </c>
       <c r="O84">
-        <v>0.44541976872900002</v>
+        <v>1.2078298601300001E-2</v>
       </c>
       <c r="P84">
-        <v>1.2078298601300001E-2</v>
+        <v>986669</v>
       </c>
       <c r="Q84">
-        <v>986669</v>
+        <v>73762</v>
       </c>
       <c r="R84">
-        <v>73762</v>
+        <v>84729</v>
       </c>
       <c r="S84">
-        <v>84729</v>
+        <v>6485.3223684200002</v>
       </c>
       <c r="T84">
-        <v>6485.3223684200002</v>
+        <v>6899.7832167799997</v>
       </c>
       <c r="U84">
-        <v>6899.7832167799997</v>
+        <v>12093</v>
       </c>
       <c r="V84">
-        <v>12093</v>
-      </c>
-      <c r="W84">
         <v>13366</v>
       </c>
     </row>
-    <row r="85" spans="1:23">
+    <row r="85" spans="1:22">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -6773,34 +6521,31 @@
         <v>0.95087853314199999</v>
       </c>
       <c r="O85">
-        <v>0.59650957621199996</v>
+        <v>2.5598606298599998E-2</v>
       </c>
       <c r="P85">
-        <v>2.5598606298599998E-2</v>
+        <v>1699196</v>
       </c>
       <c r="Q85">
-        <v>1699196</v>
+        <v>94631</v>
       </c>
       <c r="R85">
         <v>94631</v>
       </c>
       <c r="S85">
-        <v>94631</v>
+        <v>8538.2211055299995</v>
       </c>
       <c r="T85">
-        <v>8538.2211055299995</v>
+        <v>8943.1368421099996</v>
       </c>
       <c r="U85">
-        <v>8943.1368421099996</v>
+        <v>22179</v>
       </c>
       <c r="V85">
         <v>22179</v>
       </c>
-      <c r="W85">
-        <v>22179</v>
-      </c>
-    </row>
-    <row r="86" spans="1:23">
+    </row>
+    <row r="86" spans="1:22">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -6844,34 +6589,31 @@
         <v>0.86613162475600003</v>
       </c>
       <c r="O86">
-        <v>0.37532897022200001</v>
+        <v>1.5759495535000001E-2</v>
       </c>
       <c r="P86">
-        <v>1.5759495535000001E-2</v>
+        <v>719819</v>
       </c>
       <c r="Q86">
-        <v>719819</v>
+        <v>30360</v>
       </c>
       <c r="R86">
         <v>30360</v>
       </c>
       <c r="S86">
-        <v>30360</v>
+        <v>6312.8947368400004</v>
       </c>
       <c r="T86">
-        <v>6312.8947368400004</v>
+        <v>6664.9907407399996</v>
       </c>
       <c r="U86">
-        <v>6664.9907407399996</v>
+        <v>9324</v>
       </c>
       <c r="V86">
-        <v>9324</v>
-      </c>
-      <c r="W86">
         <v>10015</v>
       </c>
     </row>
-    <row r="87" spans="1:23">
+    <row r="87" spans="1:22">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -6915,34 +6657,31 @@
         <v>0.94132773365199995</v>
       </c>
       <c r="O87">
-        <v>0.65448731850399999</v>
+        <v>2.3139771071300001E-2</v>
       </c>
       <c r="P87">
-        <v>2.3139771071300001E-2</v>
+        <v>3657827</v>
       </c>
       <c r="Q87">
-        <v>3657827</v>
+        <v>14461</v>
       </c>
       <c r="R87">
         <v>14461</v>
       </c>
       <c r="S87">
-        <v>14461</v>
+        <v>2323.1429478999999</v>
       </c>
       <c r="T87">
-        <v>2323.1429478999999</v>
+        <v>2469.8359216700001</v>
       </c>
       <c r="U87">
-        <v>2469.8359216700001</v>
+        <v>2632</v>
       </c>
       <c r="V87">
-        <v>2632</v>
-      </c>
-      <c r="W87">
         <v>2753</v>
       </c>
     </row>
-    <row r="88" spans="1:23">
+    <row r="88" spans="1:22">
       <c r="A88" t="s">
         <v>86</v>
       </c>
@@ -6986,34 +6725,31 @@
         <v>0.94682887135799998</v>
       </c>
       <c r="O88">
-        <v>0.41563998563799998</v>
+        <v>2.0117957843900001E-2</v>
       </c>
       <c r="P88">
-        <v>2.0117957843900001E-2</v>
+        <v>1881491</v>
       </c>
       <c r="Q88">
-        <v>1881491</v>
+        <v>31260</v>
       </c>
       <c r="R88">
         <v>31260</v>
       </c>
       <c r="S88">
-        <v>31260</v>
+        <v>3797.8282828299998</v>
       </c>
       <c r="T88">
-        <v>3797.8282828299998</v>
+        <v>4028.8886509600002</v>
       </c>
       <c r="U88">
-        <v>4028.8886509600002</v>
+        <v>6077</v>
       </c>
       <c r="V88">
-        <v>6077</v>
-      </c>
-      <c r="W88">
         <v>6345</v>
       </c>
     </row>
-    <row r="89" spans="1:23">
+    <row r="89" spans="1:22">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -7057,30 +6793,27 @@
         <v>0.94088024695799999</v>
       </c>
       <c r="O89">
-        <v>0.38838365211699999</v>
+        <v>1.6511255864900001E-2</v>
       </c>
       <c r="P89">
-        <v>1.6511255864900001E-2</v>
+        <v>1001628</v>
       </c>
       <c r="Q89">
-        <v>1001628</v>
+        <v>11022</v>
       </c>
       <c r="R89">
         <v>11022</v>
       </c>
       <c r="S89">
-        <v>11022</v>
+        <v>2434.35766423</v>
       </c>
       <c r="T89">
-        <v>2434.35766423</v>
+        <v>2548.6717557299999</v>
       </c>
       <c r="U89">
-        <v>2548.6717557299999</v>
+        <v>2743</v>
       </c>
       <c r="V89">
-        <v>2743</v>
-      </c>
-      <c r="W89">
         <v>3187</v>
       </c>
     </row>

</xml_diff>